<commit_message>
tidying on Inv 2018 data
</commit_message>
<xml_diff>
--- a/_meta/data-raw/Fields_Formulas_GHGInv1.xlsx
+++ b/_meta/data-raw/Fields_Formulas_GHGInv1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://metcmn-my.sharepoint.com/personal/laine_mcnamara_metc_state_mn_us/Documents/Documents/Other general support/GHG-CPRG/GHG Inv v1 workbooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\ghg-cprg\_meta\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="8_{2C43D6A5-C73F-4F6A-9C9F-B46C8AA27C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{961A655A-7BBA-4C39-AC5A-4CAABF961D9D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F17F93-38D1-44CE-99B8-E5FB800F8E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{03B76BE8-F7F8-4BA1-A5C0-284EEBC79998}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{03B76BE8-F7F8-4BA1-A5C0-284EEBC79998}"/>
   </bookViews>
   <sheets>
     <sheet name="field_names" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="89">
   <si>
     <t>Abc Sort</t>
   </si>
@@ -267,12 +267,6 @@
     <t>Activity</t>
   </si>
   <si>
-    <t>Y?</t>
-  </si>
-  <si>
-    <t>Activity?</t>
-  </si>
-  <si>
     <t>File name</t>
   </si>
   <si>
@@ -325,6 +319,12 @@
   </si>
   <si>
     <t>C:\github\ghg.inv.app\01_ghg_inventory\0102_transportation\0102_on_road\commercial_vehicles\data\output</t>
+  </si>
+  <si>
+    <t>Metadata</t>
+  </si>
+  <si>
+    <t>Demographics</t>
   </si>
 </sst>
 </file>
@@ -360,12 +360,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -684,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{349EA80B-F151-4857-9ACD-1F2011CD5C7E}">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -720,6 +717,9 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="C4" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -728,6 +728,9 @@
       <c r="B5" t="s">
         <v>43</v>
       </c>
+      <c r="C5" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -736,6 +739,9 @@
       <c r="B6" t="s">
         <v>43</v>
       </c>
+      <c r="C6" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -754,6 +760,9 @@
       <c r="B9" t="s">
         <v>43</v>
       </c>
+      <c r="C9" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -919,16 +928,22 @@
       <c r="A30" t="s">
         <v>28</v>
       </c>
+      <c r="B30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="C31" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -950,11 +965,23 @@
       <c r="A35" t="s">
         <v>33</v>
       </c>
+      <c r="B35" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>34</v>
       </c>
+      <c r="B36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
@@ -976,15 +1003,33 @@
       <c r="A39" t="s">
         <v>37</v>
       </c>
+      <c r="B39" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>38</v>
       </c>
+      <c r="B40" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>43</v>
+      </c>
+      <c r="C41" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -1023,7 +1068,7 @@
       <c r="A2" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1122,16 +1167,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" t="s">
         <v>72</v>
       </c>
-      <c r="C1" t="s">
-        <v>74</v>
-      </c>
       <c r="D1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E1" t="s">
         <v>7</v>
@@ -1139,16 +1184,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" t="s">
         <v>73</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>76</v>
-      </c>
-      <c r="C2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D2" t="s">
-        <v>78</v>
       </c>
       <c r="E2">
         <v>2018</v>
@@ -1156,16 +1201,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" t="s">
         <v>76</v>
-      </c>
-      <c r="C3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D3" t="s">
-        <v>78</v>
       </c>
       <c r="E3">
         <v>2018</v>
@@ -1173,16 +1218,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" t="s">
         <v>76</v>
-      </c>
-      <c r="C4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D4" t="s">
-        <v>78</v>
       </c>
       <c r="E4">
         <v>2019</v>
@@ -1190,16 +1235,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" t="s">
         <v>82</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>83</v>
-      </c>
-      <c r="C5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D5" t="s">
-        <v>85</v>
       </c>
       <c r="E5">
         <v>2018</v>
@@ -1207,16 +1252,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" t="s">
         <v>86</v>
       </c>
-      <c r="B6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C6" t="s">
-        <v>88</v>
-      </c>
       <c r="D6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E6">
         <v>2018</v>

</xml_diff>